<commit_message>
Add Birth Registration feature to HDS Explorer - allow resumeMode arg on FormUtil - update PregnancyRegistration to create pregnancies for Outcome - fix code generation for multiple members
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="26265" windowHeight="13155" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
     <t>group</t>
   </si>
@@ -208,13 +208,16 @@
     <t>3.3.1. Especifique o local onde ocorreu o parto</t>
   </si>
   <si>
+    <t>${birthPlace}='OTHER'</t>
+  </si>
+  <si>
     <t>childs</t>
   </si>
   <si>
     <t>start repeat</t>
   </si>
   <si>
-    <t>${numberOfOutcomes}</t>
+    <t>$child_outcomes</t>
   </si>
   <si>
     <t>5. Relationships of Members with the new Head of Household</t>
@@ -244,6 +247,9 @@
     <t>5.2. Código da criança</t>
   </si>
   <si>
+    <t>${outcomeType}='LBR'</t>
+  </si>
+  <si>
     <t>childName</t>
   </si>
   <si>
@@ -484,9 +490,6 @@
     <t>Aborto induzido</t>
   </si>
   <si>
-    <t>birthingPlace</t>
-  </si>
-  <si>
     <t>HOME</t>
   </si>
   <si>
@@ -538,6 +541,15 @@
     <t>form_name::pt</t>
   </si>
   <si>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>repeat_name</t>
+  </si>
+  <si>
+    <t>xml_node_name</t>
+  </si>
+  <si>
     <t>rawPregnancyOutcome</t>
   </si>
   <si>
@@ -545,6 +557,9 @@
   </si>
   <si>
     <t>Resultado de gravidez</t>
+  </si>
+  <si>
+    <t>rawPregnancyChild</t>
   </si>
 </sst>
 </file>
@@ -552,10 +567,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -622,8 +637,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -631,7 +653,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -645,6 +667,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -653,16 +691,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,22 +706,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,38 +723,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,6 +740,27 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -762,7 +777,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,55 +792,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,127 +954,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,6 +1001,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -991,39 +1021,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1054,6 +1051,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1068,145 +1080,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1216,7 +1237,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1260,6 +1281,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1270,23 +1292,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1603,8 +1621,8 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1612,15 +1630,15 @@
     <col min="1" max="1" width="12.9142857142857" customWidth="1"/>
     <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="22.247619047619" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="19.9904761904762" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20" style="17" customWidth="1"/>
+    <col min="6" max="6" width="19.9904761904762" style="18" customWidth="1"/>
+    <col min="7" max="7" width="24.0761904761905" style="18" customWidth="1"/>
     <col min="8" max="8" width="51.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="11" width="16.352380952381" customWidth="1"/>
     <col min="12" max="12" width="9.28571428571429" customWidth="1"/>
-    <col min="14" max="14" width="31" customWidth="1"/>
+    <col min="14" max="14" width="31" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1640,10 +1658,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1664,7 +1682,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="18" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1677,13 +1695,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -1697,7 +1715,7 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="17"/>
+      <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -1705,15 +1723,15 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="18" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="19" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
@@ -1727,7 +1745,7 @@
       <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="17"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -1739,16 +1757,16 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" t="s">
         <v>25</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1766,16 +1784,16 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1793,16 +1811,16 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
@@ -1820,16 +1838,16 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -1837,7 +1855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="13" customHeight="1" spans="1:12">
+    <row r="8" ht="13" customHeight="1" spans="1:13">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
         <v>36</v>
@@ -1845,17 +1863,20 @@
       <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
       <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1867,16 +1888,16 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
       <c r="H9" t="s">
         <v>42</v>
       </c>
       <c r="I9" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1889,23 +1910,23 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="25"/>
       <c r="H10" t="s">
         <v>47</v>
       </c>
       <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
       <c r="L10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" ht="12" customHeight="1" spans="1:14">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
         <v>49</v>
@@ -1913,235 +1934,250 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
       <c r="H11" t="s">
         <v>50</v>
       </c>
       <c r="I11" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="N11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" s="17" customFormat="1" spans="1:15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="F12" s="26"/>
+      <c r="G12" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="H12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="I12" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="21"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>58</v>
+      <c r="F13" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+        <v>61</v>
+      </c>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
       <c r="L13" t="b">
         <v>1</v>
       </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
-      <c r="D14" t="s">
-        <v>61</v>
+      <c r="D14" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
+        <v>64</v>
+      </c>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
       <c r="L14" t="b">
         <v>1</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="N14" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="H15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I15" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>68</v>
+      <c r="F16" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+        <v>72</v>
+      </c>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
       <c r="L16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="N16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
+        <v>75</v>
+      </c>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
       <c r="L17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
-      <c r="D18" t="s">
-        <v>74</v>
+      <c r="D18" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
+        <v>80</v>
+      </c>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
       <c r="L18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="N18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" s="17" customFormat="1" spans="1:15">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+        <v>81</v>
+      </c>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>84</v>
-      </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
+        <v>86</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
       <c r="L20" t="b">
         <v>1</v>
       </c>
@@ -2151,22 +2187,22 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I21" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+        <v>90</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
       <c r="L21" t="b">
         <v>1</v>
       </c>
@@ -2176,22 +2212,22 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I22" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+        <v>93</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
       <c r="L22" t="b">
         <v>1</v>
       </c>
@@ -2201,23 +2237,23 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1"/>
@@ -2265,7 +2301,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A19" sqref="A19:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2281,7 +2317,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2295,317 +2331,317 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="10" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="10" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="10" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="10" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2740,39 +2776,59 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="28.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="29.7142857142857" customWidth="1"/>
+    <col min="4" max="5" width="12.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Validation Rules on Pregnancy Registration and Outcome
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="13155" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -1621,8 +1621,8 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Add Support for editing HDS Core Forms
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="10740" tabRatio="500"/>
+    <workbookView windowWidth="29655" windowHeight="10605" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
   <si>
     <t>group</t>
   </si>
@@ -247,9 +247,6 @@
     <t>5.2. Código da criança</t>
   </si>
   <si>
-    <t>${outcomeType}='LBR'</t>
-  </si>
-  <si>
     <t>childName</t>
   </si>
   <si>
@@ -368,6 +365,18 @@
   </si>
   <si>
     <t>Feminino</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Not Known</t>
+  </si>
+  <si>
+    <t>Desconhecido</t>
+  </si>
+  <si>
+    <t>${outcomeType}!='LBR'</t>
   </si>
   <si>
     <t>HOH</t>
@@ -567,10 +576,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -615,14 +624,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -638,7 +639,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,14 +682,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -676,51 +701,20 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -737,22 +731,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -760,7 +769,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -786,13 +795,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,13 +855,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,61 +873,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,91 +963,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,11 +1010,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1027,26 +1042,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,6 +1060,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1083,161 +1090,163 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1246,6 +1255,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1278,6 +1293,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1288,23 +1307,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1621,8 +1639,8 @@
   <sheetPr/>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F16" sqref="$A16:$XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1632,8 +1650,8 @@
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="22.247619047619" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="19.9904761904762" style="18" customWidth="1"/>
-    <col min="7" max="7" width="24.0761904761905" style="18" customWidth="1"/>
+    <col min="6" max="6" width="19.9904761904762" style="22" customWidth="1"/>
+    <col min="7" max="7" width="24.0761904761905" style="22" customWidth="1"/>
     <col min="8" max="8" width="51.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="11" width="16.352380952381" customWidth="1"/>
@@ -1658,10 +1676,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1682,7 +1700,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="22" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1695,13 +1713,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="23" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -1715,7 +1733,7 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="18"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -1723,15 +1741,15 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="19" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
@@ -1745,7 +1763,7 @@
       <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="18"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -1757,16 +1775,16 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" t="s">
         <v>25</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1784,16 +1802,16 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1811,16 +1829,16 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
@@ -1838,16 +1856,16 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -1863,16 +1881,16 @@
       <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -1888,16 +1906,16 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" t="s">
         <v>42</v>
       </c>
       <c r="I9" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1910,18 +1928,18 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="28"/>
       <c r="H10" t="s">
         <v>47</v>
       </c>
       <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
       <c r="L10" t="b">
         <v>1</v>
       </c>
@@ -1934,16 +1952,16 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
       <c r="H11" t="s">
         <v>50</v>
       </c>
       <c r="I11" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
@@ -1951,46 +1969,46 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" s="17" customFormat="1" spans="1:15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
+    <row r="12" s="21" customFormat="1" spans="1:15">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="21"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="25"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="25"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" t="s">
         <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="22" t="s">
         <v>59</v>
       </c>
       <c r="H13" t="s">
@@ -1999,17 +2017,17 @@
       <c r="I13" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
       <c r="L13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24" t="s">
+    <row r="14" spans="1:13">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E14" t="s">
@@ -2021,163 +2039,148 @@
       <c r="I14" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
       <c r="L14" t="b">
         <v>1</v>
       </c>
       <c r="M14" t="b">
         <v>1</v>
       </c>
-      <c r="N14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" t="s">
-        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="H15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" t="s">
         <v>67</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" t="s">
         <v>68</v>
-      </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" t="s">
-        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
         <v>70</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>71</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" t="s">
         <v>72</v>
-      </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" t="b">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" t="s">
-        <v>73</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
       </c>
       <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" t="s">
         <v>74</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" t="b">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24" t="s">
+      <c r="E18" t="s">
         <v>76</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="H18" t="s">
         <v>78</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>79</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" s="21" customFormat="1" spans="1:15">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" s="17" customFormat="1" spans="1:15">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="21"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="25"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
         <v>82</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>84</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>85</v>
       </c>
-      <c r="I20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
       <c r="L20" t="b">
         <v>1</v>
       </c>
@@ -2187,22 +2190,22 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>88</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>89</v>
       </c>
-      <c r="I21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
       <c r="L21" t="b">
         <v>1</v>
       </c>
@@ -2212,22 +2215,22 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
         <v>17</v>
       </c>
       <c r="H22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" t="s">
         <v>92</v>
       </c>
-      <c r="I22" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
       <c r="L22" t="b">
         <v>1</v>
       </c>
@@ -2237,23 +2240,23 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1"/>
@@ -2298,26 +2301,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="13.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="25.8571428571429" style="1" customWidth="1"/>
     <col min="3" max="4" width="32.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="13.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="21.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2328,274 +2332,281 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F1" s="18" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
         <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="16" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="20" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7" t="s">
+      <c r="B18" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="9" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D20" t="s">
@@ -2603,13 +2614,13 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="14" t="s">
         <v>153</v>
       </c>
       <c r="D21" t="s">
@@ -2617,13 +2628,13 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="14" t="s">
         <v>156</v>
       </c>
       <c r="D22" t="s">
@@ -2631,140 +2642,152 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
         <v>159</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="10"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="10"/>
-      <c r="E25" s="12"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="4"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12"/>
+      <c r="A26" s="12"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="12"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="16"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="4"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="12"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="4"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="12"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="39" spans="5:5">
-      <c r="E39" s="12"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
     </row>
     <row r="40" spans="5:5">
-      <c r="E40" s="12"/>
+      <c r="E40" s="14"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="12"/>
+      <c r="E41" s="14"/>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" s="14"/>
     </row>
     <row r="43" spans="5:5">
-      <c r="E43" s="12"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="5:5">
-      <c r="E44" s="12"/>
+      <c r="E44" s="14"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="12"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="12"/>
+      <c r="E46" s="14"/>
     </row>
     <row r="47" spans="5:5">
-      <c r="E47" s="12"/>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2793,33 +2816,33 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2828,7 +2851,7 @@
         <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow registration of Deaths out of Pregnancy Outcomes
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29655" windowHeight="10605" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="21045" windowHeight="6555" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -367,10 +367,10 @@
     <t>Feminino</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Not Known</t>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
   <si>
     <t>Desconhecido</t>
@@ -576,10 +576,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -624,6 +624,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -632,30 +640,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -678,14 +663,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
@@ -694,29 +671,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -730,16 +692,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,7 +732,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -769,7 +747,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -807,187 +807,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,15 +998,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1021,6 +1012,65 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1043,210 +1093,160 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1291,9 +1291,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1650,8 +1647,8 @@
     <col min="3" max="3" width="14.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="22.247619047619" customWidth="1"/>
     <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="19.9904761904762" style="22" customWidth="1"/>
-    <col min="7" max="7" width="24.0761904761905" style="22" customWidth="1"/>
+    <col min="6" max="6" width="19.9904761904762" style="21" customWidth="1"/>
+    <col min="7" max="7" width="24.0761904761905" style="21" customWidth="1"/>
     <col min="8" max="8" width="51.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="11" width="16.352380952381" customWidth="1"/>
@@ -1676,10 +1673,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1700,7 +1697,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1713,13 +1710,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
@@ -1733,7 +1730,7 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="22"/>
+      <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -1741,15 +1738,15 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="23" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="22" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
@@ -1763,7 +1760,7 @@
       <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="22"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -1775,16 +1772,16 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" t="s">
         <v>25</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1802,16 +1799,16 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1829,16 +1826,16 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
@@ -1856,16 +1853,16 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
@@ -1881,16 +1878,16 @@
       <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -1906,16 +1903,16 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" t="s">
         <v>42</v>
       </c>
       <c r="I9" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1928,18 +1925,18 @@
       <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="27"/>
       <c r="H10" t="s">
         <v>47</v>
       </c>
       <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
       <c r="L10" t="b">
         <v>1</v>
       </c>
@@ -1952,16 +1949,16 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" t="s">
         <v>50</v>
       </c>
       <c r="I11" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
       <c r="L11" t="b">
         <v>1</v>
       </c>
@@ -1969,46 +1966,46 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" s="21" customFormat="1" spans="1:15">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25" t="s">
+    <row r="12" s="20" customFormat="1" spans="1:15">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29" t="s">
+      <c r="F12" s="28"/>
+      <c r="G12" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="25"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="25"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" t="s">
         <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>59</v>
       </c>
       <c r="H13" t="s">
@@ -2017,17 +2014,17 @@
       <c r="I13" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
       <c r="L13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="19" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="18" t="s">
         <v>62</v>
       </c>
       <c r="E14" t="s">
@@ -2039,8 +2036,8 @@
       <c r="I14" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
       <c r="L14" t="b">
         <v>1</v>
       </c>
@@ -2049,9 +2046,9 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" t="s">
         <v>65</v>
       </c>
@@ -2064,23 +2061,23 @@
       <c r="I15" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
       <c r="L15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" t="s">
         <v>68</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="21" t="s">
         <v>69</v>
       </c>
       <c r="H16" t="s">
@@ -2089,16 +2086,16 @@
       <c r="I16" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
       <c r="L16" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" t="s">
         <v>72</v>
       </c>
@@ -2111,23 +2108,23 @@
       <c r="I17" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
       <c r="L17" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="19" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="18" t="s">
         <v>75</v>
       </c>
       <c r="E18" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>77</v>
       </c>
       <c r="H18" t="s">
@@ -2136,32 +2133,32 @@
       <c r="I18" t="s">
         <v>79</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
       <c r="L18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" s="21" customFormat="1" spans="1:15">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25" t="s">
+    <row r="19" s="20" customFormat="1" spans="1:15">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="25"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="24"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
@@ -2179,8 +2176,8 @@
       <c r="I20" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
       <c r="L20" t="b">
         <v>1</v>
       </c>
@@ -2204,8 +2201,8 @@
       <c r="I21" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
       <c r="L21" t="b">
         <v>1</v>
       </c>
@@ -2229,8 +2226,8 @@
       <c r="I22" t="s">
         <v>92</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
       <c r="L22" t="b">
         <v>1</v>
       </c>
@@ -2240,23 +2237,23 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1"/>
@@ -2304,7 +2301,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2332,7 +2329,7 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2410,7 +2407,7 @@
         <v>107</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2427,7 +2424,7 @@
       <c r="D7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Default server Url
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14055" tabRatio="500"/>
+    <workbookView windowWidth="28650" windowHeight="12045" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -711,12 +711,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -754,36 +754,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -796,10 +770,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -818,6 +799,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -827,7 +823,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -841,8 +837,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,13 +854,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -871,10 +861,32 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -886,33 +898,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -960,175 +949,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1176,7 +1165,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1192,6 +1181,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1228,8 +1226,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1243,166 +1243,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1472,9 +1461,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1792,7 +1780,7 @@
   <sheetPr/>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J26" sqref="A5:J26"/>
     </sheetView>
   </sheetViews>
@@ -2158,11 +2146,11 @@
       <c r="I12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
       <c r="M12" s="25" t="b">
         <v>1</v>
       </c>
@@ -2311,7 +2299,7 @@
       <c r="I18" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="30" t="s">
         <v>97</v>
       </c>
       <c r="K18" s="28"/>
@@ -2334,9 +2322,9 @@
       <c r="G19" s="26"/>
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
       <c r="O19" s="24"/>
@@ -2491,8 +2479,8 @@
   <sheetPr/>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
Fix Delete Form Extension CollectedData when deleting CoreCollectedData
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/pregnancy_outcome_form.xlsx
+++ b/app/src/main/res/raw/pregnancy_outcome_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25830" windowHeight="9885" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="18045" windowHeight="6825" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="238">
   <si>
     <t>group</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>4.3. Nom de l'enfant</t>
+  </si>
+  <si>
+    <t>${outcomeType} = 'LBR'</t>
   </si>
   <si>
     <t>childGender</t>
@@ -768,10 +771,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -819,8 +822,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -834,23 +846,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,29 +864,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -903,17 +883,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -925,16 +897,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -949,7 +913,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,6 +923,45 @@
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -994,13 +997,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,97 +1045,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1120,13 +1069,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,7 +1141,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,13 +1153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,13 +1165,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1296,54 +1299,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1361,10 +1316,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1388,153 +1341,203 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1965,8 +1968,8 @@
   <sheetPr/>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1982,7 +1985,7 @@
     <col min="9" max="9" width="55" customWidth="1"/>
     <col min="10" max="10" width="48.1619047619048" customWidth="1"/>
     <col min="11" max="12" width="16.2666666666667" customWidth="1"/>
-    <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
+    <col min="13" max="13" width="26.9333333333333" customWidth="1"/>
     <col min="15" max="15" width="31" style="1" customWidth="1"/>
     <col min="16" max="16" width="13.4571428571429" customWidth="1"/>
   </cols>
@@ -2453,29 +2456,29 @@
       </c>
       <c r="K16" s="37"/>
       <c r="L16" s="37"/>
-      <c r="M16" t="b">
-        <v>1</v>
+      <c r="M16" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1"/>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
@@ -2486,19 +2489,19 @@
     <row r="18" spans="1:13">
       <c r="A18" s="1"/>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K18" s="37"/>
       <c r="L18" s="37"/>
@@ -2509,22 +2512,22 @@
     <row r="19" spans="1:13">
       <c r="A19" s="1"/>
       <c r="D19" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K19" s="37"/>
       <c r="L19" s="37"/>
@@ -2540,7 +2543,7 @@
         <v>65</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
@@ -2556,26 +2559,26 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="27" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
       <c r="H21" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
@@ -2591,26 +2594,26 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
       <c r="H22" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K22" s="39"/>
       <c r="L22" s="39"/>
@@ -2626,26 +2629,26 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K23" s="39"/>
       <c r="L23" s="39"/>
@@ -2661,12 +2664,12 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>19</v>
@@ -2674,13 +2677,13 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K24" s="39"/>
       <c r="L24" s="39"/>
@@ -2696,12 +2699,12 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>19</v>
@@ -2709,13 +2712,13 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K25" s="39"/>
       <c r="L25" s="39"/>
@@ -2731,12 +2734,12 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>19</v>
@@ -2744,13 +2747,13 @@
       <c r="F26" s="35"/>
       <c r="G26" s="35"/>
       <c r="H26" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -2829,8 +2832,8 @@
   <sheetPr/>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75"/>
@@ -2848,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2874,251 +2877,251 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3126,16 +3129,16 @@
         <v>72</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3143,16 +3146,16 @@
         <v>72</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3160,16 +3163,16 @@
         <v>72</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3177,16 +3180,16 @@
         <v>72</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3194,16 +3197,16 @@
         <v>56</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3211,16 +3214,16 @@
         <v>56</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3228,16 +3231,16 @@
         <v>56</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3245,33 +3248,33 @@
         <v>56</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3279,16 +3282,16 @@
         <v>56</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3296,16 +3299,16 @@
         <v>56</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3470,39 +3473,39 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3511,7 +3514,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>